<commit_message>
Fir in the hole
</commit_message>
<xml_diff>
--- a/statergy.xlsx
+++ b/statergy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kiran/Documents/GitHub/Leet-Code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A801830D-BC40-D940-A3B6-7F5D382CED04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF1D10C8-A902-784C-BA9D-13C55C273195}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16200" activeTab="5" xr2:uid="{3D71AE53-AE20-0444-BFDD-F4EE28B54982}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="122">
   <si>
     <t>Problems</t>
   </si>
@@ -746,6 +746,43 @@
   </si>
   <si>
     <t>https://www.youtube.com/watch?v=JdCj9bAX8tQ&amp;ab_channel=AyushiSharma</t>
+  </si>
+  <si>
+    <t>LC 1758</t>
+  </si>
+  <si>
+    <t>Measy</t>
+  </si>
+  <si>
+    <t>Maximum Changes to Binary</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> * - The function iterates over each character in the string 's'.
+ * - It counts the number of changes needed to make the string follow two patterns: "010101..." and "101010...".
+ * - 'count0' is used to track the number of changes needed for the "010101..." pattern.
+ *   - For even indices (0, 2, 4, ...), the expected character is '0'.
+ *   - For odd indices (1, 3, 5, ...), the expected character is '1'.
+ * - 'count1' is used to track the number of changes needed for the "101010..." pattern.
+ *   - For even indices, the expected character is '1'.
+ *   - For odd indices, the expected character is '0'.
+ * - The function returns the minimum of 'count0' and 'count1', indicating the least number of changes needed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LC </t>
+  </si>
+  <si>
+    <t>Valid Soduku</t>
+  </si>
+  <si>
+    <t>// Approach:
+// 1. Use three 2D arrays (rows, colm, and box) to track the numbers present in each row, column, and 3x3 sub-box.
+// 2. Iterate through each cell in the board.
+//    - Convert the character at board[i][j] to an integer index (0-8) if it's not '.'.
+//    - Calculate the index of the 3x3 sub-box.
+//    - Check if the number already exists in the corresponding row, column, and sub-box.
+//      - If it does, return false (invalid Sudoku).
+//    - Otherwise, mark the number as seen in the corresponding row, column, and sub-box.
+// 3. If no duplicates are found, return true (valid Sudoku).</t>
   </si>
 </sst>
 </file>
@@ -1704,10 +1741,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B30F7361-C0E3-9E4B-BA46-FF3FE1D175A7}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1811,6 +1848,34 @@
         <v>114</v>
       </c>
     </row>
+    <row r="8" spans="1:7" ht="187" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>115</v>
+      </c>
+      <c r="B8" t="s">
+        <v>116</v>
+      </c>
+      <c r="C8" t="s">
+        <v>117</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="170" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>119</v>
+      </c>
+      <c r="B9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" t="s">
+        <v>120</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G5" r:id="rId1" xr:uid="{37C1BBFD-1B4A-A543-B984-DEC3083B165E}"/>

</xml_diff>